<commit_message>
update buscas price change
</commit_message>
<xml_diff>
--- a/buscas.xlsx
+++ b/buscas.xlsx
@@ -346,8 +346,8 @@
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3">
-        <v>4000.0</v>
+      <c r="C3" s="2">
+        <v>2500.0</v>
       </c>
       <c r="D3" s="3">
         <v>4500.0</v>

</xml_diff>